<commit_message>
Country report script drafted
</commit_message>
<xml_diff>
--- a/Inputs/Wellcome grants.xlsx
+++ b/Inputs/Wellcome grants.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/Project MODARI/Phase 2 - Implementation/2) Awards/Wellcome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{C52ECE99-6C0E-4DF0-A33F-FDD70B5BF136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A10A0C1C-25F5-479D-BC30-6770049509A8}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{C52ECE99-6C0E-4DF0-A33F-FDD70B5BF136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BB560C9-73D3-4C0D-82EA-D6E39D117814}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A966BEC5-38D6-46D6-8317-0837EF3A602D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A966BEC5-38D6-46D6-8317-0837EF3A602D}"/>
   </bookViews>
   <sheets>
     <sheet name="Wellcome ODA grants" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="595">
   <si>
     <t>Internal ID</t>
   </si>
@@ -2014,6 +2014,18 @@
   </si>
   <si>
     <t>ODA funding</t>
+  </si>
+  <si>
+    <t>220121/Z/20/Z</t>
+  </si>
+  <si>
+    <t>UMURINZI - Unprecedented Movement to drive a Unified Rwandan Initiative for National ZEBOVAC Immunization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ongoing outbreak of Ebola Virus Disease (EVD) in the Democratic Republic of Congo (DRC) is of particular concern for the Government of Rwanda, when one considers the high population density of Rwanda and the number of people crossing the border between Rwanda and DRC on a daily basis. Janssen Vaccines and Prevention B. V. (Janssen) and the Rwanda Ministry of Health have recently entered into an agreement for a donation of 200,000 doses of the Ad26.ZEBOV and MVA-BN-Filo Ebola vaccine. Rwanda FDA has granted conditional approval of the vaccine under exceptional emergency circumstances in accordance with SAGE recommendations to put in place approvals for investigational medicines and vaccines as an immediate priority for preparedness.
+This Ebola vaccine initiative consists of: 1) a mass vaccination campaign that will target up to 193,000 individuals crossing or living in sectors/districts sharing the border with DRC; this program is known as UMURINZI (Unprecedented Movement to drive a Unified Rwandan Initiative for National ZEBOVAC Immunization); 2) a clinical trial to evaluate the immunogenicity of the vaccine regimen in 2,000 people; 3) and a clinical trial to evaluate the safety of the vaccine among 5,000 pregnant women.
+This proposal concerns start up of UMURINZI only.
+</t>
   </si>
 </sst>
 </file>
@@ -2432,28 +2444,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E9CF53-AB8B-4026-B76F-F3B62C915F7B}">
-  <dimension ref="A1:Q126"/>
+  <dimension ref="A1:Q127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.3984375" style="1" customWidth="1"/>
-    <col min="7" max="10" width="12.59765625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.59765625" customWidth="1"/>
-    <col min="12" max="17" width="12.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.375" style="1" customWidth="1"/>
+    <col min="7" max="10" width="12.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.625" customWidth="1"/>
+    <col min="12" max="17" width="12.625" style="1" customWidth="1"/>
     <col min="18" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2506,7 +2518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>179</v>
       </c>
@@ -2541,14 +2553,14 @@
         <v>750000</v>
       </c>
       <c r="P2" s="5">
-        <f>O2-N2</f>
+        <f t="shared" ref="P2:P33" si="0">O2-N2</f>
         <v>0</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>180</v>
       </c>
@@ -2583,14 +2595,14 @@
         <v>4160408.5</v>
       </c>
       <c r="P3" s="5">
-        <f>O3-N3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>181</v>
       </c>
@@ -2625,14 +2637,14 @@
         <v>800000</v>
       </c>
       <c r="P4" s="5">
-        <f>O4-N4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>174</v>
       </c>
@@ -2667,14 +2679,14 @@
         <v>1097432</v>
       </c>
       <c r="P5" s="5">
-        <f>O5-N5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>175</v>
       </c>
@@ -2709,14 +2721,14 @@
         <v>1909721</v>
       </c>
       <c r="P6" s="5">
-        <f>O6-N6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>176</v>
       </c>
@@ -2751,14 +2763,14 @@
         <v>555800</v>
       </c>
       <c r="P7" s="5">
-        <f>O7-N7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>177</v>
       </c>
@@ -2793,14 +2805,14 @@
         <v>1444200</v>
       </c>
       <c r="P8" s="5">
-        <f>O8-N8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>178</v>
       </c>
@@ -2835,14 +2847,14 @@
         <v>267206</v>
       </c>
       <c r="P9" s="5">
-        <f>O9-N9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>138</v>
       </c>
@@ -2877,14 +2889,14 @@
         <v>3817668.17</v>
       </c>
       <c r="P10" s="5">
-        <f>O10-N10</f>
+        <f t="shared" si="0"/>
         <v>1908834.0799999998</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>182</v>
       </c>
@@ -2922,14 +2934,14 @@
         <v>0</v>
       </c>
       <c r="P11" s="5">
-        <f>O11-N11</f>
+        <f t="shared" si="0"/>
         <v>-17659614.699999999</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>183</v>
       </c>
@@ -2967,14 +2979,14 @@
         <v>0</v>
       </c>
       <c r="P12" s="5">
-        <f>O12-N12</f>
+        <f t="shared" si="0"/>
         <v>-17917773</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>184</v>
       </c>
@@ -3012,14 +3024,14 @@
         <v>0</v>
       </c>
       <c r="P13" s="5">
-        <f>O13-N13</f>
+        <f t="shared" si="0"/>
         <v>-9264935</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>185</v>
       </c>
@@ -3054,14 +3066,14 @@
         <v>3564939.94</v>
       </c>
       <c r="P14" s="5">
-        <f>O14-N14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>186</v>
       </c>
@@ -3096,14 +3108,14 @@
         <v>214927</v>
       </c>
       <c r="P15" s="5">
-        <f>O15-N15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>187</v>
       </c>
@@ -3138,14 +3150,14 @@
         <v>222047</v>
       </c>
       <c r="P16" s="5">
-        <f>O16-N16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>188</v>
       </c>
@@ -3180,14 +3192,14 @@
         <v>137264</v>
       </c>
       <c r="P17" s="5">
-        <f>O17-N17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>189</v>
       </c>
@@ -3222,14 +3234,14 @@
         <v>348589</v>
       </c>
       <c r="P18" s="5">
-        <f>O18-N18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>190</v>
       </c>
@@ -3264,14 +3276,14 @@
         <v>134785</v>
       </c>
       <c r="P19" s="5">
-        <f>O19-N19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>191</v>
       </c>
@@ -3306,14 +3318,14 @@
         <v>242334</v>
       </c>
       <c r="P20" s="5">
-        <f>O20-N20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>192</v>
       </c>
@@ -3348,14 +3360,14 @@
         <v>351726</v>
       </c>
       <c r="P21" s="5">
-        <f>O21-N21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>193</v>
       </c>
@@ -3390,14 +3402,14 @@
         <v>68564</v>
       </c>
       <c r="P22" s="5">
-        <f>O22-N22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -3438,14 +3450,14 @@
         <v>5138215</v>
       </c>
       <c r="P23" s="5">
-        <f>O23-N23</f>
+        <f t="shared" si="0"/>
         <v>4816500</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>194</v>
       </c>
@@ -3480,14 +3492,14 @@
         <v>111539</v>
       </c>
       <c r="P24" s="5">
-        <f>O24-N24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>195</v>
       </c>
@@ -3525,14 +3537,14 @@
         <v>108422</v>
       </c>
       <c r="P25" s="5">
-        <f>O25-N25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>196</v>
       </c>
@@ -3567,14 +3579,14 @@
         <v>132017</v>
       </c>
       <c r="P26" s="5">
-        <f>O26-N26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>197</v>
       </c>
@@ -3609,14 +3621,14 @@
         <v>132017</v>
       </c>
       <c r="P27" s="5">
-        <f>O27-N27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>198</v>
       </c>
@@ -3651,14 +3663,14 @@
         <v>161148</v>
       </c>
       <c r="P28" s="5">
-        <f>O28-N28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>199</v>
       </c>
@@ -3693,14 +3705,14 @@
         <v>16805</v>
       </c>
       <c r="P29" s="5">
-        <f>O29-N29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>200</v>
       </c>
@@ -3735,14 +3747,14 @@
         <v>799989.3</v>
       </c>
       <c r="P30" s="5">
-        <f>O30-N30</f>
+        <f t="shared" si="0"/>
         <v>799989.3</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>139</v>
       </c>
@@ -3775,14 +3787,14 @@
         <v>0</v>
       </c>
       <c r="P31" s="5">
-        <f>O31-N31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q31" s="1" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>201</v>
       </c>
@@ -3815,14 +3827,14 @@
         <v>0</v>
       </c>
       <c r="P32" s="5">
-        <f>O32-N32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q32" s="1" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>202</v>
       </c>
@@ -3857,14 +3869,14 @@
         <v>349103</v>
       </c>
       <c r="P33" s="5">
-        <f>O33-N33</f>
+        <f t="shared" si="0"/>
         <v>349103</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>203</v>
       </c>
@@ -3899,14 +3911,14 @@
         <v>500000</v>
       </c>
       <c r="P34" s="5">
-        <f>O34-N34</f>
+        <f t="shared" ref="P34:P65" si="1">O34-N34</f>
         <v>250000</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>204</v>
       </c>
@@ -3944,14 +3956,14 @@
         <v>174945.94</v>
       </c>
       <c r="P35" s="5">
-        <f>O35-N35</f>
+        <f t="shared" si="1"/>
         <v>87472.97</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
@@ -3989,14 +4001,14 @@
         <v>7838</v>
       </c>
       <c r="P36" s="5">
-        <f>O36-N36</f>
+        <f t="shared" si="1"/>
         <v>3920</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>205</v>
       </c>
@@ -4034,14 +4046,14 @@
         <v>311973.84999999998</v>
       </c>
       <c r="P37" s="5">
-        <f>O37-N37</f>
+        <f t="shared" si="1"/>
         <v>155986.91999999998</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>206</v>
       </c>
@@ -4076,14 +4088,14 @@
         <v>3914598.95</v>
       </c>
       <c r="P38" s="5">
-        <f>O38-N38</f>
+        <f t="shared" si="1"/>
         <v>2968263.1100000003</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>119</v>
       </c>
@@ -4118,14 +4130,14 @@
         <v>3099568</v>
       </c>
       <c r="P39" s="5">
-        <f>O39-N39</f>
+        <f t="shared" si="1"/>
         <v>248140</v>
       </c>
       <c r="Q39" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>207</v>
       </c>
@@ -4160,14 +4172,14 @@
         <v>38701</v>
       </c>
       <c r="P40" s="5">
-        <f>O40-N40</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q40" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>213</v>
       </c>
@@ -4200,14 +4212,14 @@
         <v>483800</v>
       </c>
       <c r="P41" s="5">
-        <f>O41-N41</f>
+        <f t="shared" si="1"/>
         <v>241900</v>
       </c>
       <c r="Q41" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>214</v>
       </c>
@@ -4242,14 +4254,14 @@
         <v>40187.01</v>
       </c>
       <c r="P42" s="5">
-        <f>O42-N42</f>
+        <f t="shared" si="1"/>
         <v>20093.500000000004</v>
       </c>
       <c r="Q42" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>151</v>
       </c>
@@ -4284,14 +4296,14 @@
         <v>1724966</v>
       </c>
       <c r="P43" s="5">
-        <f>O43-N43</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q43" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>148</v>
       </c>
@@ -4326,14 +4338,14 @@
         <v>2411528</v>
       </c>
       <c r="P44" s="5">
-        <f>O44-N44</f>
+        <f t="shared" si="1"/>
         <v>2068247</v>
       </c>
       <c r="Q44" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>208</v>
       </c>
@@ -4368,14 +4380,14 @@
         <v>600000</v>
       </c>
       <c r="P45" s="5">
-        <f>O45-N45</f>
+        <f t="shared" si="1"/>
         <v>300000</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>149</v>
       </c>
@@ -4413,14 +4425,14 @@
         <v>3812875</v>
       </c>
       <c r="P46" s="5">
-        <f>O46-N46</f>
+        <f t="shared" si="1"/>
         <v>1906437.5</v>
       </c>
       <c r="Q46" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>125</v>
       </c>
@@ -4455,14 +4467,14 @@
         <v>373072.7</v>
       </c>
       <c r="P47" s="5">
-        <f>O47-N47</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q47" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>121</v>
       </c>
@@ -4500,14 +4512,14 @@
         <v>349998.83</v>
       </c>
       <c r="P48" s="5">
-        <f>O48-N48</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q48" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>120</v>
       </c>
@@ -4542,14 +4554,14 @@
         <v>1008647.39</v>
       </c>
       <c r="P49" s="5">
-        <f>O49-N49</f>
+        <f t="shared" si="1"/>
         <v>1008647.39</v>
       </c>
       <c r="Q49" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>124</v>
       </c>
@@ -4587,14 +4599,14 @@
         <v>578609.35</v>
       </c>
       <c r="P50" s="5">
-        <f>O50-N50</f>
+        <f t="shared" si="1"/>
         <v>565328.04999999993</v>
       </c>
       <c r="Q50" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>123</v>
       </c>
@@ -4632,14 +4644,14 @@
         <v>582464.21</v>
       </c>
       <c r="P51" s="5">
-        <f>O51-N51</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q51" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>209</v>
       </c>
@@ -4674,14 +4686,14 @@
         <v>328985.56</v>
       </c>
       <c r="P52" s="5">
-        <f>O52-N52</f>
+        <f t="shared" si="1"/>
         <v>328985.56</v>
       </c>
       <c r="Q52" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>48</v>
       </c>
@@ -4719,14 +4731,14 @@
         <v>1599263</v>
       </c>
       <c r="P53" s="5">
-        <f>O53-N53</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q53" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>210</v>
       </c>
@@ -4761,14 +4773,14 @@
         <v>585582.56999999995</v>
       </c>
       <c r="P54" s="5">
-        <f>O54-N54</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q54" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>126</v>
       </c>
@@ -4803,14 +4815,14 @@
         <v>413535.64</v>
       </c>
       <c r="P55" s="5">
-        <f>O55-N55</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>211</v>
       </c>
@@ -4848,14 +4860,14 @@
         <v>85000</v>
       </c>
       <c r="P56" s="5">
-        <f>O56-N56</f>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="Q56" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>122</v>
       </c>
@@ -4890,14 +4902,14 @@
         <v>334409</v>
       </c>
       <c r="P57" s="5">
-        <f>O57-N57</f>
+        <f t="shared" si="1"/>
         <v>334409</v>
       </c>
       <c r="Q57" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>212</v>
       </c>
@@ -4932,14 +4944,14 @@
         <v>257630</v>
       </c>
       <c r="P58" s="5">
-        <f>O58-N58</f>
+        <f t="shared" si="1"/>
         <v>257630</v>
       </c>
       <c r="Q58" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>128</v>
       </c>
@@ -4977,14 +4989,14 @@
         <v>653307.67000000004</v>
       </c>
       <c r="P59" s="5">
-        <f>O59-N59</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q59" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>127</v>
       </c>
@@ -5019,14 +5031,14 @@
         <v>1588565</v>
       </c>
       <c r="P60" s="5">
-        <f>O60-N60</f>
+        <f t="shared" si="1"/>
         <v>1588565</v>
       </c>
       <c r="Q60" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>147</v>
       </c>
@@ -5064,14 +5076,14 @@
         <v>186305.14</v>
       </c>
       <c r="P61" s="5">
-        <f>O61-N61</f>
+        <f t="shared" si="1"/>
         <v>93152.57</v>
       </c>
       <c r="Q61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>54</v>
       </c>
@@ -5115,14 +5127,14 @@
         <v>318672</v>
       </c>
       <c r="P62" s="5">
-        <f>O62-N62</f>
+        <f t="shared" si="1"/>
         <v>159336</v>
       </c>
       <c r="Q62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>144</v>
       </c>
@@ -5157,14 +5169,14 @@
         <v>343006</v>
       </c>
       <c r="P63" s="5">
-        <f>O63-N63</f>
+        <f t="shared" si="1"/>
         <v>168377</v>
       </c>
       <c r="Q63" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>146</v>
       </c>
@@ -5199,14 +5211,14 @@
         <v>304066</v>
       </c>
       <c r="P64" s="5">
-        <f>O64-N64</f>
+        <f t="shared" si="1"/>
         <v>152033</v>
       </c>
       <c r="Q64" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>145</v>
       </c>
@@ -5244,14 +5256,14 @@
         <v>728291</v>
       </c>
       <c r="P65" s="5">
-        <f>O65-N65</f>
+        <f t="shared" si="1"/>
         <v>364145</v>
       </c>
       <c r="Q65" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>150</v>
       </c>
@@ -5289,14 +5301,14 @@
         <v>4016242</v>
       </c>
       <c r="P66" s="5">
-        <f>O66-N66</f>
+        <f t="shared" ref="P66:P98" si="2">O66-N66</f>
         <v>2008121</v>
       </c>
       <c r="Q66" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>159</v>
       </c>
@@ -5334,14 +5346,14 @@
         <v>3687583</v>
       </c>
       <c r="P67" s="5">
-        <f>O67-N67</f>
+        <f t="shared" si="2"/>
         <v>1885328</v>
       </c>
       <c r="Q67" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>143</v>
       </c>
@@ -5379,14 +5391,14 @@
         <v>120000</v>
       </c>
       <c r="P68" s="5">
-        <f>O68-N68</f>
+        <f t="shared" si="2"/>
         <v>60000</v>
       </c>
       <c r="Q68" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>142</v>
       </c>
@@ -5421,14 +5433,14 @@
         <v>120000</v>
       </c>
       <c r="P69" s="5">
-        <f>O69-N69</f>
+        <f t="shared" si="2"/>
         <v>60000</v>
       </c>
       <c r="Q69" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>141</v>
       </c>
@@ -5463,14 +5475,14 @@
         <v>120000</v>
       </c>
       <c r="P70" s="5">
-        <f>O70-N70</f>
+        <f t="shared" si="2"/>
         <v>60000</v>
       </c>
       <c r="Q70" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>140</v>
       </c>
@@ -5505,14 +5517,14 @@
         <v>120000</v>
       </c>
       <c r="P71" s="5">
-        <f>O71-N71</f>
+        <f t="shared" si="2"/>
         <v>60000</v>
       </c>
       <c r="Q71" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>153</v>
       </c>
@@ -5550,14 +5562,14 @@
         <v>307623.67</v>
       </c>
       <c r="P72" s="5">
-        <f>O72-N72</f>
+        <f t="shared" si="2"/>
         <v>153811.66999999998</v>
       </c>
       <c r="Q72" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>161</v>
       </c>
@@ -5595,14 +5607,14 @@
         <v>195361</v>
       </c>
       <c r="P73" s="5">
-        <f>O73-N73</f>
+        <f t="shared" si="2"/>
         <v>97680.5</v>
       </c>
       <c r="Q73" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>154</v>
       </c>
@@ -5637,14 +5649,14 @@
         <v>336054</v>
       </c>
       <c r="P74" s="5">
-        <f>O74-N74</f>
+        <f t="shared" si="2"/>
         <v>168027</v>
       </c>
       <c r="Q74" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>155</v>
       </c>
@@ -5682,14 +5694,14 @@
         <v>766354</v>
       </c>
       <c r="P75" s="5">
-        <f>O75-N75</f>
+        <f t="shared" si="2"/>
         <v>383177</v>
       </c>
       <c r="Q75" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>156</v>
       </c>
@@ -5727,14 +5739,14 @@
         <v>720067</v>
       </c>
       <c r="P76" s="5">
-        <f>O76-N76</f>
+        <f t="shared" si="2"/>
         <v>360034</v>
       </c>
       <c r="Q76" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>215</v>
       </c>
@@ -5769,14 +5781,14 @@
         <v>2063517</v>
       </c>
       <c r="P77" s="5">
-        <f>O77-N77</f>
+        <f t="shared" si="2"/>
         <v>1650813</v>
       </c>
       <c r="Q77" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>158</v>
       </c>
@@ -5814,14 +5826,14 @@
         <v>3803801</v>
       </c>
       <c r="P78" s="5">
-        <f>O78-N78</f>
+        <f t="shared" si="2"/>
         <v>1901900</v>
       </c>
       <c r="Q78" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>157</v>
       </c>
@@ -5859,14 +5871,14 @@
         <v>1600709</v>
       </c>
       <c r="P79" s="5">
-        <f>O79-N79</f>
+        <f t="shared" si="2"/>
         <v>800354.5</v>
       </c>
       <c r="Q79" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>216</v>
       </c>
@@ -5901,14 +5913,14 @@
         <v>56063.01</v>
       </c>
       <c r="P80" s="5">
-        <f>O80-N80</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q80" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>217</v>
       </c>
@@ -5943,14 +5955,14 @@
         <v>75161</v>
       </c>
       <c r="P81" s="5">
-        <f>O81-N81</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q81" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>152</v>
       </c>
@@ -5985,14 +5997,14 @@
         <v>120000</v>
       </c>
       <c r="P82" s="5">
-        <f>O82-N82</f>
+        <f t="shared" si="2"/>
         <v>60000</v>
       </c>
       <c r="Q82" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>163</v>
       </c>
@@ -6025,14 +6037,14 @@
         <v>0</v>
       </c>
       <c r="P83" s="5">
-        <f>O83-N83</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q83" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>160</v>
       </c>
@@ -6067,14 +6079,14 @@
         <v>120000</v>
       </c>
       <c r="P84" s="5">
-        <f>O84-N84</f>
+        <f t="shared" si="2"/>
         <v>60000</v>
       </c>
       <c r="Q84" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>218</v>
       </c>
@@ -6112,16 +6124,16 @@
         <v>542290.44999999995</v>
       </c>
       <c r="P85" s="5">
-        <f>O85-N85</f>
+        <f t="shared" si="2"/>
         <v>542290.44999999995</v>
       </c>
       <c r="Q85" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>219</v>
+        <v>592</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>313</v>
@@ -6136,43 +6148,43 @@
         <v>471</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>406</v>
+        <v>593</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>582</v>
+        <v>594</v>
       </c>
       <c r="L86" s="2">
-        <v>43836</v>
+        <v>43752</v>
       </c>
       <c r="M86" s="2">
-        <v>44445</v>
+        <v>43935</v>
       </c>
       <c r="N86" s="5">
-        <v>1510287.88</v>
+        <v>405745</v>
       </c>
       <c r="O86" s="5">
-        <v>3325532.71</v>
+        <v>405745</v>
       </c>
       <c r="P86" s="5">
-        <f>O86-N86</f>
-        <v>1815244.83</v>
+        <f t="shared" ref="P86" si="3">O86-N86</f>
+        <v>0</v>
       </c>
       <c r="Q86" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>471</v>
@@ -6181,118 +6193,118 @@
         <v>406</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="L87" s="2">
-        <v>43800</v>
+        <v>43836</v>
       </c>
       <c r="M87" s="2">
-        <v>44409</v>
+        <v>44445</v>
       </c>
       <c r="N87" s="5">
-        <v>184755</v>
+        <v>1510287.88</v>
       </c>
       <c r="O87" s="5">
-        <v>369503.6</v>
+        <v>3325532.71</v>
       </c>
       <c r="P87" s="5">
-        <f>O87-N87</f>
-        <v>184748.59999999998</v>
+        <f t="shared" si="2"/>
+        <v>1815244.83</v>
       </c>
       <c r="Q87" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="L88" s="2">
+        <v>43800</v>
+      </c>
+      <c r="M88" s="2">
+        <v>44409</v>
+      </c>
+      <c r="N88" s="5">
+        <v>184755</v>
+      </c>
+      <c r="O88" s="5">
+        <v>369503.6</v>
+      </c>
+      <c r="P88" s="5">
+        <f t="shared" si="2"/>
+        <v>184748.59999999998</v>
+      </c>
+      <c r="Q88" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A89" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E89" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="F88" s="1" t="s">
+      <c r="F89" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G88" s="1" t="s">
+      <c r="G89" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H88" s="1" t="s">
+      <c r="H89" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="J88" s="1" t="s">
+      <c r="J89" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="K88" s="1" t="s">
+      <c r="K89" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="L88" s="2">
+      <c r="L89" s="2">
         <v>44075</v>
       </c>
-      <c r="M88" s="2">
+      <c r="M89" s="2">
         <v>45900</v>
       </c>
-      <c r="N88" s="5">
+      <c r="N89" s="5">
         <v>1140173</v>
       </c>
-      <c r="O88" s="5">
+      <c r="O89" s="5">
         <v>2280346</v>
       </c>
-      <c r="P88" s="5">
-        <f>O88-N88</f>
+      <c r="P89" s="5">
+        <f t="shared" si="2"/>
         <v>1140173</v>
       </c>
-      <c r="Q88" s="1" t="s">
+      <c r="Q89" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A89" s="6" t="s">
+    <row r="90" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A90" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="J89" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="K89" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="L89" s="2">
-        <v>43770</v>
-      </c>
-      <c r="M89" s="2">
-        <v>44500</v>
-      </c>
-      <c r="N89" s="5">
-        <v>4059969.16</v>
-      </c>
-      <c r="O89" s="5">
-        <v>5358273.1399999997</v>
-      </c>
-      <c r="P89" s="5">
-        <f>O89-N89</f>
-        <v>1298303.9799999995</v>
-      </c>
-      <c r="Q89" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A90" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>315</v>
@@ -6319,520 +6331,520 @@
         <v>44500</v>
       </c>
       <c r="N90" s="5">
-        <v>0</v>
+        <v>4059969.16</v>
       </c>
       <c r="O90" s="5">
-        <v>1701696.02</v>
+        <v>5358273.1399999997</v>
       </c>
       <c r="P90" s="5">
-        <f>O90-N90</f>
-        <v>1701696.02</v>
+        <f t="shared" si="2"/>
+        <v>1298303.9799999995</v>
       </c>
       <c r="Q90" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="L91" s="2">
+        <v>43770</v>
+      </c>
+      <c r="M91" s="2">
+        <v>44500</v>
+      </c>
+      <c r="N91" s="5">
+        <v>0</v>
+      </c>
+      <c r="O91" s="5">
+        <v>1701696.02</v>
+      </c>
+      <c r="P91" s="5">
+        <f t="shared" si="2"/>
+        <v>1701696.02</v>
+      </c>
+      <c r="Q91" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A92" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E92" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F91" s="1" t="s">
+      <c r="F92" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="G91" s="1" t="s">
+      <c r="G92" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="J91" s="1" t="s">
+      <c r="J92" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="K91" s="1" t="s">
+      <c r="K92" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="L91" s="2">
+      <c r="L92" s="2">
         <v>44105</v>
       </c>
-      <c r="M91" s="2">
+      <c r="M92" s="2">
         <v>45930</v>
       </c>
-      <c r="N91" s="5">
+      <c r="N92" s="5">
         <v>292294</v>
       </c>
-      <c r="O91" s="5">
+      <c r="O92" s="5">
         <v>584588</v>
       </c>
-      <c r="P91" s="5">
-        <f>O91-N91</f>
+      <c r="P92" s="5">
+        <f t="shared" si="2"/>
         <v>292294</v>
-      </c>
-      <c r="Q91" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A92" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="J92" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="K92" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="L92" s="2">
-        <v>44075</v>
-      </c>
-      <c r="M92" s="2">
-        <v>45169</v>
-      </c>
-      <c r="N92" s="5">
-        <v>103661</v>
-      </c>
-      <c r="O92" s="5">
-        <v>207323</v>
-      </c>
-      <c r="P92" s="5">
-        <f>O92-N92</f>
-        <v>103662</v>
       </c>
       <c r="Q92" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="L93" s="2">
+        <v>44075</v>
+      </c>
+      <c r="M93" s="2">
+        <v>45169</v>
+      </c>
+      <c r="N93" s="5">
+        <v>103661</v>
+      </c>
+      <c r="O93" s="5">
+        <v>207323</v>
+      </c>
+      <c r="P93" s="5">
+        <f t="shared" si="2"/>
+        <v>103662</v>
+      </c>
+      <c r="Q93" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A94" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F93" s="1" t="s">
+      <c r="E94" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="J93" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="K93" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="L93" s="2">
-        <v>43910</v>
-      </c>
-      <c r="M93" s="2">
-        <v>44396</v>
-      </c>
-      <c r="N93" s="5">
-        <v>124963</v>
-      </c>
-      <c r="O93" s="5">
-        <v>249926</v>
-      </c>
-      <c r="P93" s="5">
-        <f>O93-N93</f>
-        <v>124963</v>
-      </c>
-      <c r="Q93" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A94" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>453</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>505</v>
+        <v>486</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L94" s="2">
-        <v>43895</v>
+        <v>43910</v>
       </c>
       <c r="M94" s="2">
-        <v>44259</v>
+        <v>44396</v>
       </c>
       <c r="N94" s="5">
-        <v>0</v>
+        <v>124963</v>
       </c>
       <c r="O94" s="5">
-        <v>888104</v>
+        <v>249926</v>
       </c>
       <c r="P94" s="5">
-        <f>O94-N94</f>
-        <v>888104</v>
+        <f t="shared" si="2"/>
+        <v>124963</v>
       </c>
       <c r="Q94" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>168</v>
+        <v>224</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>277</v>
+        <v>317</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>34</v>
+        <v>453</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H95" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="J95" s="1" t="s">
-        <v>371</v>
+        <v>409</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>551</v>
+        <v>586</v>
       </c>
       <c r="L95" s="2">
-        <v>44075</v>
+        <v>43895</v>
       </c>
       <c r="M95" s="2">
-        <v>45535</v>
+        <v>44259</v>
       </c>
       <c r="N95" s="5">
-        <v>859476.5</v>
+        <v>0</v>
       </c>
       <c r="O95" s="5">
-        <v>1718953</v>
+        <v>888104</v>
       </c>
       <c r="P95" s="5">
-        <f>O95-N95</f>
-        <v>859476.5</v>
+        <f t="shared" si="2"/>
+        <v>888104</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>103</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>437</v>
+        <v>34</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="L96" s="2">
-        <v>44200</v>
+        <v>44075</v>
       </c>
       <c r="M96" s="2">
-        <v>45660</v>
+        <v>45535</v>
       </c>
       <c r="N96" s="5">
-        <v>1395744</v>
+        <v>859476.5</v>
       </c>
       <c r="O96" s="5">
-        <v>2791488</v>
+        <v>1718953</v>
       </c>
       <c r="P96" s="5">
-        <f>O96-N96</f>
-        <v>1395744</v>
+        <f t="shared" si="2"/>
+        <v>859476.5</v>
       </c>
       <c r="Q96" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>103</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>34</v>
+        <v>437</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="L97" s="2">
-        <v>44197</v>
+        <v>44200</v>
       </c>
       <c r="M97" s="2">
-        <v>45657</v>
+        <v>45660</v>
       </c>
       <c r="N97" s="5">
-        <v>1776461.5</v>
+        <v>1395744</v>
       </c>
       <c r="O97" s="5">
-        <v>3552923</v>
+        <v>2791488</v>
       </c>
       <c r="P97" s="5">
-        <f>O97-N97</f>
-        <v>1776461.5</v>
+        <f t="shared" si="2"/>
+        <v>1395744</v>
       </c>
       <c r="Q97" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H98" s="1" t="s">
-        <v>481</v>
-      </c>
       <c r="J98" s="1" t="s">
-        <v>334</v>
+        <v>373</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>517</v>
+        <v>553</v>
       </c>
       <c r="L98" s="2">
-        <v>44018</v>
+        <v>44197</v>
       </c>
       <c r="M98" s="2">
-        <v>44754</v>
+        <v>45657</v>
       </c>
       <c r="N98" s="5">
-        <v>0</v>
+        <v>1776461.5</v>
       </c>
       <c r="O98" s="5">
-        <v>646963</v>
+        <v>3552923</v>
       </c>
       <c r="P98" s="5">
-        <f>O98-N98</f>
-        <v>646963</v>
+        <f t="shared" si="2"/>
+        <v>1776461.5</v>
       </c>
       <c r="Q98" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L99" s="2">
-        <v>43956</v>
+        <v>44018</v>
       </c>
       <c r="M99" s="2">
-        <v>44685</v>
+        <v>44754</v>
       </c>
       <c r="N99" s="5">
-        <v>864564</v>
+        <v>0</v>
       </c>
       <c r="O99" s="5">
-        <v>864564</v>
+        <v>646963</v>
       </c>
       <c r="P99" s="5">
-        <f>O99-N99</f>
-        <v>0</v>
+        <f t="shared" ref="P99:P130" si="4">O99-N99</f>
+        <v>646963</v>
       </c>
       <c r="Q99" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>422</v>
+        <v>21</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L100" s="2">
-        <v>43978</v>
+        <v>43956</v>
       </c>
       <c r="M100" s="2">
-        <v>44707</v>
+        <v>44685</v>
       </c>
       <c r="N100" s="5">
+        <v>864564</v>
+      </c>
+      <c r="O100" s="5">
+        <v>864564</v>
+      </c>
+      <c r="P100" s="5">
+        <f t="shared" si="4"/>
         <v>0</v>
-      </c>
-      <c r="O100" s="5">
-        <v>1030349</v>
-      </c>
-      <c r="P100" s="5">
-        <f>O100-N100</f>
-        <v>1030349</v>
       </c>
       <c r="Q100" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>46</v>
+        <v>422</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="L101" s="2">
-        <v>44013</v>
+        <v>43978</v>
       </c>
       <c r="M101" s="2">
-        <v>44742</v>
+        <v>44707</v>
       </c>
       <c r="N101" s="5">
-        <v>755818.12</v>
+        <v>0</v>
       </c>
       <c r="O101" s="5">
-        <v>1217834</v>
+        <v>1030349</v>
       </c>
       <c r="P101" s="5">
-        <f>O101-N101</f>
-        <v>462015.88</v>
+        <f t="shared" si="4"/>
+        <v>1030349</v>
       </c>
       <c r="Q101" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>421</v>
+        <v>46</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>70</v>
+        <v>14</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>484</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="L102" s="2">
         <v>44013</v>
@@ -6841,349 +6853,349 @@
         <v>44742</v>
       </c>
       <c r="N102" s="5">
-        <v>2003681</v>
+        <v>755818.12</v>
       </c>
       <c r="O102" s="5">
-        <v>2003681</v>
+        <v>1217834</v>
       </c>
       <c r="P102" s="5">
-        <f>O102-N102</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>462015.88</v>
       </c>
       <c r="Q102" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>458</v>
+        <v>70</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="L103" s="2">
-        <v>44056</v>
+        <v>44013</v>
       </c>
       <c r="M103" s="2">
-        <v>44785</v>
+        <v>44742</v>
       </c>
       <c r="N103" s="5">
-        <v>1416424</v>
+        <v>2003681</v>
       </c>
       <c r="O103" s="5">
-        <v>1416424</v>
+        <v>2003681</v>
       </c>
       <c r="P103" s="5">
-        <f>O103-N103</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q103" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="H104" s="1" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="L104" s="2">
-        <v>44044</v>
+        <v>44056</v>
       </c>
       <c r="M104" s="2">
-        <v>44773</v>
+        <v>44785</v>
       </c>
       <c r="N104" s="5">
-        <v>399361.71</v>
+        <v>1416424</v>
       </c>
       <c r="O104" s="5">
-        <v>823389.75</v>
+        <v>1416424</v>
       </c>
       <c r="P104" s="5">
-        <f>O104-N104</f>
-        <v>424028.04</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="Q104" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
-        <v>225</v>
+        <v>135</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>318</v>
+        <v>244</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>40</v>
+        <v>424</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>14</v>
+        <v>459</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>485</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>410</v>
+        <v>339</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>587</v>
+        <v>522</v>
       </c>
       <c r="L105" s="2">
-        <v>43931</v>
+        <v>44044</v>
       </c>
       <c r="M105" s="2">
-        <v>44478</v>
+        <v>44773</v>
       </c>
       <c r="N105" s="5">
-        <v>0</v>
+        <v>399361.71</v>
       </c>
       <c r="O105" s="5">
-        <v>184142</v>
+        <v>823389.75</v>
       </c>
       <c r="P105" s="5">
-        <f>O105-N105</f>
-        <v>184142</v>
+        <f t="shared" si="4"/>
+        <v>424028.04</v>
       </c>
       <c r="Q105" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
-        <v>17</v>
+    <row r="106" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A106" s="6" t="s">
+        <v>225</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>20</v>
+        <v>318</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>22</v>
+        <v>410</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>110</v>
+        <v>587</v>
       </c>
       <c r="L106" s="2">
-        <v>43937</v>
+        <v>43931</v>
       </c>
       <c r="M106" s="2">
-        <v>44135</v>
+        <v>44478</v>
       </c>
       <c r="N106" s="5">
-        <v>96664</v>
+        <v>0</v>
       </c>
       <c r="O106" s="5">
-        <v>96664</v>
+        <v>184142</v>
       </c>
       <c r="P106" s="5">
-        <f>O106-N106</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>184142</v>
       </c>
       <c r="Q106" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A107" s="6" t="s">
-        <v>226</v>
+    <row r="107" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>312</v>
+        <v>18</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>449</v>
+        <v>21</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>470</v>
+        <v>14</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>411</v>
+        <v>22</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>588</v>
+        <v>110</v>
       </c>
       <c r="L107" s="2">
-        <v>43931</v>
+        <v>43937</v>
       </c>
       <c r="M107" s="2">
-        <v>44296</v>
+        <v>44135</v>
       </c>
       <c r="N107" s="5">
-        <v>1000000</v>
+        <v>96664</v>
       </c>
       <c r="O107" s="5">
-        <v>2000000.01</v>
+        <v>96664</v>
       </c>
       <c r="P107" s="5">
-        <f>O107-N107</f>
-        <v>1000000.01</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="Q107" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="L108" s="2">
+        <v>43931</v>
+      </c>
+      <c r="M108" s="2">
+        <v>44296</v>
+      </c>
+      <c r="N108" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="O108" s="5">
+        <v>2000000.01</v>
+      </c>
+      <c r="P108" s="5">
+        <f t="shared" si="4"/>
+        <v>1000000.01</v>
+      </c>
+      <c r="Q108" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A109" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="E109" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="F108" s="1" t="s">
+      <c r="F109" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J108" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="K108" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="L108" s="2">
-        <v>44109</v>
-      </c>
-      <c r="M108" s="2">
-        <v>44838</v>
-      </c>
-      <c r="N108" s="5">
-        <v>142915</v>
-      </c>
-      <c r="O108" s="5">
-        <v>285830</v>
-      </c>
-      <c r="P108" s="5">
-        <f>O108-N108</f>
-        <v>142915</v>
-      </c>
-      <c r="Q108" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="109" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A109" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="L109" s="2">
-        <v>44084</v>
+        <v>44109</v>
       </c>
       <c r="M109" s="2">
-        <v>44994</v>
+        <v>44838</v>
       </c>
       <c r="N109" s="5">
-        <v>60000</v>
+        <v>142915</v>
       </c>
       <c r="O109" s="5">
-        <v>120000</v>
+        <v>285830</v>
       </c>
       <c r="P109" s="5">
-        <f>O109-N109</f>
-        <v>60000</v>
+        <f t="shared" si="4"/>
+        <v>142915</v>
       </c>
       <c r="Q109" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>103</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>434</v>
+        <v>34</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L110" s="2">
-        <v>44129</v>
+        <v>44084</v>
       </c>
       <c r="M110" s="2">
-        <v>45040</v>
+        <v>44994</v>
       </c>
       <c r="N110" s="5">
         <v>60000</v>
@@ -7192,64 +7204,64 @@
         <v>120000</v>
       </c>
       <c r="P110" s="5">
-        <f>O110-N110</f>
+        <f t="shared" si="4"/>
         <v>60000</v>
       </c>
       <c r="Q110" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="L111" s="2">
+        <v>44129</v>
+      </c>
+      <c r="M111" s="2">
+        <v>45040</v>
+      </c>
+      <c r="N111" s="5">
+        <v>60000</v>
+      </c>
+      <c r="O111" s="5">
+        <v>120000</v>
+      </c>
+      <c r="P111" s="5">
+        <f t="shared" si="4"/>
+        <v>60000</v>
+      </c>
+      <c r="Q111" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A112" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J111" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="K111" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="L111" s="2">
-        <v>44074</v>
-      </c>
-      <c r="M111" s="2">
-        <v>44803</v>
-      </c>
-      <c r="N111" s="5">
-        <v>283840.5</v>
-      </c>
-      <c r="O111" s="5">
-        <v>567681</v>
-      </c>
-      <c r="P111" s="5">
-        <f>O111-N111</f>
-        <v>283840.5</v>
-      </c>
-      <c r="Q111" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="112" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A112" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>319</v>
-      </c>
       <c r="E112" s="1" t="s">
-        <v>321</v>
+        <v>91</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>46</v>
@@ -7258,184 +7270,175 @@
         <v>14</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>412</v>
+        <v>340</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>589</v>
+        <v>523</v>
       </c>
       <c r="L112" s="2">
-        <v>44151</v>
+        <v>44074</v>
       </c>
       <c r="M112" s="2">
-        <v>44515</v>
+        <v>44803</v>
       </c>
       <c r="N112" s="5">
-        <v>50000</v>
+        <v>283840.5</v>
       </c>
       <c r="O112" s="5">
-        <v>100000</v>
+        <v>567681</v>
       </c>
       <c r="P112" s="5">
-        <f>O112-N112</f>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>283840.5</v>
       </c>
       <c r="Q112" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="113" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>321</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>454</v>
+        <v>46</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L113" s="2">
-        <v>44136</v>
+        <v>44151</v>
       </c>
       <c r="M113" s="2">
-        <v>44500</v>
+        <v>44515</v>
       </c>
       <c r="N113" s="5">
-        <v>48135</v>
+        <v>50000</v>
       </c>
       <c r="O113" s="5">
-        <v>96270.96</v>
+        <v>100000</v>
       </c>
       <c r="P113" s="5">
-        <f>O113-N113</f>
-        <v>48135.960000000006</v>
+        <f t="shared" si="4"/>
+        <v>50000</v>
       </c>
       <c r="Q113" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
-        <v>72</v>
+    <row r="114" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A114" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>75</v>
+        <v>320</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>103</v>
+        <v>321</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>76</v>
+        <v>454</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I114" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>77</v>
+        <v>413</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>111</v>
+        <v>590</v>
       </c>
       <c r="L114" s="2">
-        <v>44378</v>
+        <v>44136</v>
       </c>
       <c r="M114" s="2">
-        <v>46203</v>
+        <v>44500</v>
       </c>
       <c r="N114" s="5">
-        <v>2010416</v>
+        <v>48135</v>
       </c>
       <c r="O114" s="5">
-        <v>4020832</v>
+        <v>96270.96</v>
       </c>
       <c r="P114" s="5">
-        <f>O114-N114</f>
-        <v>2010416</v>
+        <f t="shared" si="4"/>
+        <v>48135.960000000006</v>
       </c>
       <c r="Q114" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="115" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>103</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L115" s="2">
-        <v>44440</v>
+        <v>44378</v>
       </c>
       <c r="M115" s="2">
-        <v>46265</v>
+        <v>46203</v>
       </c>
       <c r="N115" s="5">
-        <v>467629</v>
+        <v>2010416</v>
       </c>
       <c r="O115" s="5">
-        <v>935258</v>
+        <v>4020832</v>
       </c>
       <c r="P115" s="5">
-        <f>O115-N115</f>
-        <v>467629</v>
+        <f t="shared" si="4"/>
+        <v>2010416</v>
       </c>
       <c r="Q115" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="116" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>80</v>
@@ -7444,218 +7447,225 @@
         <v>103</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>85</v>
+        <v>14</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L116" s="2">
-        <v>44593</v>
+        <v>44440</v>
       </c>
       <c r="M116" s="2">
-        <v>46418</v>
+        <v>46265</v>
       </c>
       <c r="N116" s="5">
-        <v>347486</v>
+        <v>467629</v>
       </c>
       <c r="O116" s="5">
-        <v>694973</v>
+        <v>935258</v>
       </c>
       <c r="P116" s="5">
-        <f>O116-N116</f>
-        <v>347487</v>
+        <f t="shared" si="4"/>
+        <v>467629</v>
       </c>
       <c r="Q116" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="117" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>103</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H117" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I117" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L117" s="2">
-        <v>44378</v>
+        <v>44593</v>
       </c>
       <c r="M117" s="2">
-        <v>45473</v>
+        <v>46418</v>
       </c>
       <c r="N117" s="5">
-        <v>152610</v>
+        <v>347486</v>
       </c>
       <c r="O117" s="5">
-        <v>305220</v>
+        <v>694973</v>
       </c>
       <c r="P117" s="5">
-        <f>O117-N117</f>
-        <v>152610</v>
+        <f t="shared" si="4"/>
+        <v>347487</v>
       </c>
       <c r="Q117" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A118" s="6" t="s">
-        <v>173</v>
+    <row r="118" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>282</v>
+        <v>68</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>321</v>
+        <v>103</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="G118" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H118" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="I118" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="J118" s="1" t="s">
-        <v>376</v>
+        <v>71</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>556</v>
+        <v>114</v>
       </c>
       <c r="L118" s="2">
-        <v>44409</v>
+        <v>44378</v>
       </c>
       <c r="M118" s="2">
-        <v>45504</v>
-      </c>
-      <c r="N118" s="5"/>
+        <v>45473</v>
+      </c>
+      <c r="N118" s="5">
+        <v>152610</v>
+      </c>
       <c r="O118" s="5">
-        <v>315590</v>
+        <v>305220</v>
       </c>
       <c r="P118" s="5">
-        <f>O118-N118</f>
-        <v>315590</v>
+        <f t="shared" si="4"/>
+        <v>152610</v>
       </c>
       <c r="Q118" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>103</v>
+        <v>321</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>438</v>
+        <v>34</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>465</v>
+        <v>14</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="L119" s="2">
-        <v>44317</v>
+        <v>44409</v>
       </c>
       <c r="M119" s="2">
-        <v>45412</v>
+        <v>45504</v>
       </c>
       <c r="N119" s="5"/>
       <c r="O119" s="5">
-        <v>297444</v>
+        <v>315590</v>
       </c>
       <c r="P119" s="5">
-        <f>O119-N119</f>
-        <v>297444</v>
+        <f t="shared" si="4"/>
+        <v>315590</v>
       </c>
       <c r="Q119" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="6" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>246</v>
+        <v>281</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>46</v>
+        <v>438</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>14</v>
+        <v>465</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="K120" s="1"/>
+        <v>375</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>555</v>
+      </c>
       <c r="L120" s="2">
-        <v>44105</v>
+        <v>44317</v>
       </c>
       <c r="M120" s="2">
-        <v>44834</v>
+        <v>45412</v>
       </c>
       <c r="N120" s="5"/>
       <c r="O120" s="5">
-        <v>670100</v>
+        <v>297444</v>
       </c>
       <c r="P120" s="5">
-        <f>O120-N120</f>
-        <v>670100</v>
+        <f t="shared" si="4"/>
+        <v>297444</v>
       </c>
       <c r="Q120" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="121" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A121" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>20</v>
+        <v>246</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>91</v>
@@ -7666,47 +7676,37 @@
       <c r="G121" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H121" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I121" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="J121" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K121" s="1" t="s">
-        <v>115</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="K121" s="1"/>
       <c r="L121" s="2">
-        <v>44348</v>
+        <v>44105</v>
       </c>
       <c r="M121" s="2">
-        <v>44893</v>
-      </c>
-      <c r="N121" s="5">
-        <v>340531</v>
-      </c>
+        <v>44834</v>
+      </c>
+      <c r="N121" s="5"/>
       <c r="O121" s="5">
-        <v>340531</v>
+        <v>670100</v>
       </c>
       <c r="P121" s="5">
-        <f>O121-N121</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>670100</v>
       </c>
       <c r="Q121" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="122" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>20</v>
@@ -7715,151 +7715,160 @@
         <v>91</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L122" s="2">
-        <v>44287</v>
+        <v>44348</v>
       </c>
       <c r="M122" s="2">
-        <v>44651</v>
+        <v>44893</v>
       </c>
       <c r="N122" s="5">
-        <v>639793</v>
+        <v>340531</v>
       </c>
       <c r="O122" s="5">
-        <v>639793</v>
+        <v>340531</v>
       </c>
       <c r="P122" s="5">
-        <f>O122-N122</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q122" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H123" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="J123" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L123" s="2">
-        <v>44137</v>
+        <v>44287</v>
       </c>
       <c r="M123" s="2">
-        <v>44682</v>
+        <v>44651</v>
       </c>
       <c r="N123" s="5">
-        <v>331006</v>
+        <v>639793</v>
       </c>
       <c r="O123" s="5">
-        <v>662012</v>
+        <v>639793</v>
       </c>
       <c r="P123" s="5">
-        <f>O123-N123</f>
-        <v>331006</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="Q123" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="124" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>62</v>
+        <v>37</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L124" s="2">
-        <v>44350</v>
+        <v>44137</v>
       </c>
       <c r="M124" s="2">
-        <v>45079</v>
+        <v>44682</v>
       </c>
       <c r="N124" s="5">
-        <v>463888</v>
+        <v>331006</v>
       </c>
       <c r="O124" s="5">
-        <v>463888</v>
+        <v>662012</v>
       </c>
       <c r="P124" s="5">
-        <f>O124-N124</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>331006</v>
       </c>
       <c r="Q124" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="125" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>14</v>
@@ -7877,21 +7886,66 @@
         <v>45079</v>
       </c>
       <c r="N125" s="5">
+        <v>463888</v>
+      </c>
+      <c r="O125" s="5">
+        <v>463888</v>
+      </c>
+      <c r="P125" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q125" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L126" s="2">
+        <v>44350</v>
+      </c>
+      <c r="M126" s="2">
+        <v>45079</v>
+      </c>
+      <c r="N126" s="5">
         <v>492566</v>
       </c>
-      <c r="O125" s="5">
+      <c r="O126" s="5">
         <v>492566</v>
       </c>
-      <c r="P125" s="5">
-        <f>O125-N125</f>
+      <c r="P126" s="5">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q125" s="1" t="s">
+      <c r="Q126" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="126" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="K126" s="1"/>
+    <row r="127" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K127" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{A5B5B279-4815-4CD7-AA1F-478F7D49DB87}">

</xml_diff>